<commit_message>
Adding file M. Ceniuk - raport SDA.pdf with the result of the project defense and updated files with Test Cases in TestRail
</commit_message>
<xml_diff>
--- a/Test_Cases_from_TestRail/mrbuggy_7_test_cases_TestRail.xlsx
+++ b/Test_Cases_from_TestRail/mrbuggy_7_test_cases_TestRail.xlsx
@@ -15,7 +15,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="74">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="75">
   <si>
     <t>ID</t>
   </si>
@@ -107,7 +107,7 @@
     <t>C7</t>
   </si>
   <si>
-    <t>CRs- CR list filter bar in the top menu in Admin mode</t>
+    <t>CR list filter bar in the top menu in Admin mode</t>
   </si>
   <si>
     <t xml:space="preserve"> None</t>
@@ -163,7 +163,7 @@
     <t>Functional</t>
   </si>
   <si>
-    <t>9/28/2023 12:40 PM</t>
+    <t>9/28/2023 1:35 PM</t>
   </si>
   <si>
     <t>C8</t>
@@ -269,6 +269,9 @@
   </si>
   <si>
     <t>9/28/2023 1:04 PM</t>
+  </si>
+  <si>
+    <t>530s</t>
   </si>
   <si>
     <t>1. Downloaded and open MrBuggy7 desktop app.
@@ -962,29 +965,32 @@
       <c r="E5" t="s">
         <v>66</v>
       </c>
+      <c r="H5" t="s">
+        <v>67</v>
+      </c>
       <c r="K5" t="s">
-        <v>67</v>
+        <v>68</v>
       </c>
       <c r="L5" t="s">
         <v>35</v>
       </c>
       <c r="N5" t="s">
-        <v>68</v>
+        <v>69</v>
       </c>
       <c r="O5">
         <v>1</v>
       </c>
       <c r="Q5" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="S5" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="U5" t="s">
-        <v>71</v>
+        <v>72</v>
       </c>
       <c r="X5" t="s">
-        <v>72</v>
+        <v>73</v>
       </c>
       <c r="Y5" t="s">
         <v>41</v>
@@ -1002,7 +1008,7 @@
         <v>32</v>
       </c>
       <c r="AD5" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
     </row>
   </sheetData>

</xml_diff>